<commit_message>
Add GUI for input file search. Add checks for input filetypes.
</commit_message>
<xml_diff>
--- a/prod_output/sales_data.xlsx
+++ b/prod_output/sales_data.xlsx
@@ -639,7 +639,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:F161"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -650,20 +650,25 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>Suffix</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Aspect Ratio</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Units Sold</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Total Sales</t>
         </is>
@@ -677,18 +682,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>R8A7T4YJPG</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Lost Cabin Saint Jerome by Caravaggio | Print in Black Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 14.5x18.5</t>
         </is>
       </c>
-      <c r="D2" t="n">
+      <c r="E2" t="n">
         <v>3</v>
       </c>
-      <c r="E2" t="n">
+      <c r="F2" t="n">
         <v>222.97</v>
       </c>
     </row>
@@ -700,18 +710,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>3K22RLEKRG</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Lost Cabin A Dinner Table at Night by John Singer Sargent | Canvas in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 24x32 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
       <c r="E3" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
         <v>129.99</v>
       </c>
     </row>
@@ -723,18 +738,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>5JBKNNP1CW</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Lost Cabin The Artists Garden at Vetheuil by Claude Monet | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D4" t="n">
+      <c r="E4" t="n">
         <v>2</v>
       </c>
-      <c r="E4" t="n">
+      <c r="F4" t="n">
         <v>72.97999999999999</v>
       </c>
     </row>
@@ -746,18 +766,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>DW1EHLMTT4</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
           <t>Lost Cabin Camille Monet in The Garden by Claude Monet | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
       <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
         <v>64.98999999999999</v>
       </c>
     </row>
@@ -769,18 +794,23 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>7UCT5NCRBQ</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
           <t>Lost Cabin Still Life Vase with Fourteen Sunflowers by Vincent Van Gogh | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor | Image: 14x20 Frame: 20.5x26.5</t>
         </is>
       </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
       <c r="E6" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" t="n">
         <v>69.98999999999999</v>
       </c>
     </row>
@@ -792,18 +822,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>CT2HL05I87</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
           <t>Lost Cabin Red Poppies &amp; Daisies by Vincent Van Gogh | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D7" t="n">
+      <c r="E7" t="n">
         <v>4</v>
       </c>
-      <c r="E7" t="n">
+      <c r="F7" t="n">
         <v>98.95999999999999</v>
       </c>
     </row>
@@ -815,18 +850,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>E4XV1TBCO1</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
           <t>Lost Cabin Starry Night by Vincent Van Gogh | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 19x27 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D8" t="n">
+      <c r="E8" t="n">
         <v>4</v>
       </c>
-      <c r="E8" t="n">
+      <c r="F8" t="n">
         <v>272.96</v>
       </c>
     </row>
@@ -838,18 +878,23 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>CDK65AXF3P</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
           <t>Lost Cabin Road with Cypresses by Vincent Van Gogh | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 14x20 Frame: 20.5x26.5</t>
         </is>
       </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
       <c r="E9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" t="n">
         <v>69.98999999999999</v>
       </c>
     </row>
@@ -861,18 +906,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>24NVQWH4EM</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
           <t>Lost Cabin Houses with Thatched Roofs Cordeville by Vincent Van Gogh | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor | Image: 14x20 Frame: 20.5x26.5</t>
         </is>
       </c>
-      <c r="D10" t="n">
+      <c r="E10" t="n">
         <v>3</v>
       </c>
-      <c r="E10" t="n">
+      <c r="F10" t="n">
         <v>269.97</v>
       </c>
     </row>
@@ -884,18 +934,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>EQGET6UN79</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
           <t>Lost Cabin Still Life Vase with Roses by Vincent Van Gogh | Canvas in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 24x32 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D11" t="n">
-        <v>1</v>
-      </c>
       <c r="E11" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" t="n">
         <v>94.98999999999999</v>
       </c>
     </row>
@@ -907,18 +962,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>F3E33CQ7CV</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
           <t>Lost Cabin Olive Trees with Yellow Sky &amp; Sun by Vincent Van Gogh | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D12" t="n">
-        <v>1</v>
-      </c>
       <c r="E12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F12" t="n">
         <v>64.98999999999999</v>
       </c>
     </row>
@@ -930,18 +990,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>CTZXAQ5ZSN</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
           <t>Lost Cabin The Three Ages of Woman by Gustav Klimt | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D13" t="n">
-        <v>1</v>
-      </c>
       <c r="E13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F13" t="n">
         <v>64.98999999999999</v>
       </c>
     </row>
@@ -953,18 +1018,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>78HNZP9G5I</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
           <t>Lost Cabin Cattleya Orchid &amp; Three Hummingbirds by Martin Johnson Heade | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D14" t="n">
+      <c r="E14" t="n">
         <v>2</v>
       </c>
-      <c r="E14" t="n">
+      <c r="F14" t="n">
         <v>64.98999999999999</v>
       </c>
     </row>
@@ -976,18 +1046,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>GNTHAFP4AE</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
           <t>Lost Cabin Blumengarten by Gustav Klimt | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
       <c r="E15" t="n">
+        <v>1</v>
+      </c>
+      <c r="F15" t="n">
         <v>32.99</v>
       </c>
     </row>
@@ -999,18 +1074,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>7MPVIHOASR</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
           <t>Lost Cabin Coronation of the Virgin by Diego Velazquez | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D16" t="n">
+      <c r="E16" t="n">
         <v>2</v>
       </c>
-      <c r="E16" t="n">
+      <c r="F16" t="n">
         <v>134.98</v>
       </c>
     </row>
@@ -1022,18 +1102,23 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>WXXOEY0298</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
           <t>Lost Cabin The Lady of Shalott by John William Waterhouse | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D17" t="n">
+      <c r="E17" t="n">
         <v>2</v>
       </c>
-      <c r="E17" t="n">
+      <c r="F17" t="n">
         <v>57.98</v>
       </c>
     </row>
@@ -1045,18 +1130,23 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>FDELZOH4T2</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
           <t>Lost Cabin Mulberry Tree by Vincent Van Gogh | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D18" t="n">
+      <c r="E18" t="n">
         <v>4</v>
       </c>
-      <c r="E18" t="n">
+      <c r="F18" t="n">
         <v>175.96</v>
       </c>
     </row>
@@ -1068,18 +1158,23 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>QANRQE8PAH</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
           <t>Lost Cabin Vase with Red Poppies by Vincent Van Gogh | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D19" t="n">
+      <c r="E19" t="n">
         <v>5</v>
       </c>
-      <c r="E19" t="n">
+      <c r="F19" t="n">
         <v>228.95</v>
       </c>
     </row>
@@ -1091,18 +1186,23 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>ZN104BW7TY</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
           <t>Lost Cabin Haystack Under a Rainy Sky by Vincent Van Gogh | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D20" t="n">
-        <v>1</v>
-      </c>
       <c r="E20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F20" t="n">
         <v>89.98999999999999</v>
       </c>
     </row>
@@ -1114,18 +1214,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>JBMIYNO4PE</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
           <t>Lost Cabin Still Life Herring Cherries Glassware by Willem Van Aelst | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D21" t="n">
-        <v>1</v>
-      </c>
       <c r="E21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F21" t="n">
         <v>32.99</v>
       </c>
     </row>
@@ -1137,18 +1242,23 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>G57EKRJ33M</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
           <t>Lost Cabin The Proportions of The Human Figure The Vitruvian Man by Leonardo Da Vinci | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Image: 19x27 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D22" t="n">
-        <v>1</v>
-      </c>
       <c r="E22" t="n">
+        <v>1</v>
+      </c>
+      <c r="F22" t="n">
         <v>99.98999999999999</v>
       </c>
     </row>
@@ -1160,18 +1270,23 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>RETRO3-RTX60S63LQ</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
           <t>B47 Stratojet Airplane Poster Wall Art Decor Framed Print | Iconic &amp; Classic Planes Home &amp; Office Posters, Pictures &amp; Prints in Frame by Larry Grossman | Artwork Gift for Bedroom &amp; Living Room Walls</t>
         </is>
       </c>
-      <c r="D23" t="n">
-        <v>1</v>
-      </c>
       <c r="E23" t="n">
+        <v>1</v>
+      </c>
+      <c r="F23" t="n">
         <v>84.98999999999999</v>
       </c>
     </row>
@@ -1183,18 +1298,23 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>RETRO3-SKJIHEX7WI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
           <t>P40 Flying Tiger Airplane Poster Wall Art Decor Framed Print | Iconic &amp; Classic Planes Home &amp; Office Posters, Pictures &amp; Prints in Frame by Larry Grossman | Artwork for Bedroom &amp; Living Room Walls</t>
         </is>
       </c>
-      <c r="D24" t="n">
-        <v>1</v>
-      </c>
       <c r="E24" t="n">
+        <v>1</v>
+      </c>
+      <c r="F24" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -1206,18 +1326,23 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>RETRO3-2OJB5GIZF0</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
           <t>P-51 Mustang Red Tails Airplane Poster Wall Art Decor Framed Print | Iconic &amp; Classic Planes Home &amp; Office Posters, Pictures &amp; Prints by Larry Grossman | Cool Artwork for Bedroom &amp; Living Room Walls</t>
         </is>
       </c>
-      <c r="D25" t="n">
+      <c r="E25" t="n">
         <v>2</v>
       </c>
-      <c r="E25" t="n">
+      <c r="F25" t="n">
         <v>54.98</v>
       </c>
     </row>
@@ -1229,18 +1354,23 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>RETRO3-ZKJZOWUP60</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
           <t>P-40 Warhawk Airplane Poster Wall Art Decor Framed Print | Iconic &amp; Classic Planes Home &amp; Office Posters, Pictures &amp; Prints in Frame by Larry Grossman | Artwork Gift for Bedroom &amp; Living Room Walls</t>
         </is>
       </c>
-      <c r="D26" t="n">
-        <v>1</v>
-      </c>
       <c r="E26" t="n">
+        <v>1</v>
+      </c>
+      <c r="F26" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -1252,18 +1382,23 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
+          <t>RETRO3-NBRCNSK8YF</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t>Flamingo Motel Sign Poster Wall Art Decor Unframed Print | Landmarks &amp; General Photography Home &amp; Office Posters, Pictures &amp; Prints by Larry Grossman | Picture &amp; Artwork for Bedroom &amp; Living Room</t>
         </is>
       </c>
-      <c r="D27" t="n">
+      <c r="E27" t="n">
         <v>2</v>
       </c>
-      <c r="E27" t="n">
+      <c r="F27" t="n">
         <v>29.98</v>
       </c>
     </row>
@@ -1275,18 +1410,23 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>QN96LRFX92</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
           <t>Lost Cabin St George &amp; the Dragon by Raphael | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 19x27 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D28" t="n">
-        <v>1</v>
-      </c>
       <c r="E28" t="n">
+        <v>1</v>
+      </c>
+      <c r="F28" t="n">
         <v>125</v>
       </c>
     </row>
@@ -1298,18 +1438,23 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>B6KCINX0BL</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
           <t>Lost Cabin Cafe Terrace at Night by Vincent Van Gogh | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D29" t="n">
+      <c r="E29" t="n">
         <v>7</v>
       </c>
-      <c r="E29" t="n">
+      <c r="F29" t="n">
         <v>440.93</v>
       </c>
     </row>
@@ -1321,18 +1466,23 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>19R5S2KPTD</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
           <t>Lost Cabin Tamara Nun Bugatti Verde 1929 by Tamara de Lempicka | Canvas in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 24x32 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D30" t="n">
-        <v>1</v>
-      </c>
       <c r="E30" t="n">
+        <v>1</v>
+      </c>
+      <c r="F30" t="n">
         <v>129.99</v>
       </c>
     </row>
@@ -1344,18 +1494,23 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
+          <t>S9O5BYC4XQ</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>Lost Cabin Waltz by Anders Zorn | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D31" t="n">
+      <c r="E31" t="n">
         <v>3</v>
       </c>
-      <c r="E31" t="n">
+      <c r="F31" t="n">
         <v>44.97</v>
       </c>
     </row>
@@ -1367,18 +1522,23 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>2XCQEVXBS8</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Lost Cabin Among The Sierra Nevada Mountains California by Albert Bierstadt | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D32" t="n">
+      <c r="E32" t="n">
         <v>2</v>
       </c>
-      <c r="E32" t="n">
+      <c r="F32" t="n">
         <v>29.98</v>
       </c>
     </row>
@@ -1390,18 +1550,23 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
+          <t>CF7L23JLLH</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>Lost Cabin The Love Potion by Evelyn De Morgan | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D33" t="n">
-        <v>1</v>
-      </c>
       <c r="E33" t="n">
+        <v>1</v>
+      </c>
+      <c r="F33" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -1413,18 +1578,23 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
+          <t>ATPF96DL67</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>Lost Cabin Surrender of General Burgoyne by John Trumbull | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D34" t="n">
-        <v>1</v>
-      </c>
       <c r="E34" t="n">
+        <v>1</v>
+      </c>
+      <c r="F34" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -1436,18 +1606,23 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>VRQWUTP9FH</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
           <t>Lost Cabin Allegory of Sculpture by Gustav Klimt | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 14x20 Frame: 20.5x26.5</t>
         </is>
       </c>
-      <c r="D35" t="n">
-        <v>1</v>
-      </c>
       <c r="E35" t="n">
+        <v>1</v>
+      </c>
+      <c r="F35" t="n">
         <v>69.98999999999999</v>
       </c>
     </row>
@@ -1459,18 +1634,23 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
+          <t>S9QHJ5KA34</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>Lost Cabin Marooned by Howard Pyle | Canvas Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 16x24 Frame: 18x26</t>
         </is>
       </c>
-      <c r="D36" t="n">
+      <c r="E36" t="n">
         <v>3</v>
       </c>
-      <c r="E36" t="n">
+      <c r="F36" t="n">
         <v>119.97</v>
       </c>
     </row>
@@ -1482,18 +1662,23 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
+          <t>URGYCMPW1O</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Lost Cabin Declaration of Independence by John Trumbull | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D37" t="n">
-        <v>1</v>
-      </c>
       <c r="E37" t="n">
+        <v>1</v>
+      </c>
+      <c r="F37" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -1505,18 +1690,23 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
+          <t>SUWOE36OMQ</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>Lost Cabin Pinkie by Thomas Lawrence | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D38" t="n">
-        <v>1</v>
-      </c>
       <c r="E38" t="n">
+        <v>1</v>
+      </c>
+      <c r="F38" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -1528,18 +1718,23 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
+          <t>OP033P7OAS</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>Lost Cabin The Death of General Warren at the Battle of Bunker Hill by John Trumbull | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D39" t="n">
-        <v>1</v>
-      </c>
       <c r="E39" t="n">
+        <v>1</v>
+      </c>
+      <c r="F39" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -1551,18 +1746,23 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>AZZNYBKF1H</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
           <t>Pileated Woodpecker by James Audubon Framed Print Poster Wall Art Decor | Fine Artwork Painting Reproduction Posters &amp; Pictures | Gallery Prints in Wood Frame | Home &amp; Office for Bedroom &amp; Living Room</t>
         </is>
       </c>
-      <c r="D40" t="n">
-        <v>1</v>
-      </c>
       <c r="E40" t="n">
+        <v>1</v>
+      </c>
+      <c r="F40" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -1574,18 +1774,23 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>PPWG25AKB</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
           <t>Raven by James Audubon 12 x 16 Print Unframed | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Hunting Gift</t>
         </is>
       </c>
-      <c r="D41" t="n">
-        <v>1</v>
-      </c>
       <c r="E41" t="n">
+        <v>1</v>
+      </c>
+      <c r="F41" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -1597,18 +1802,23 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>RXH1XWF1SN</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
           <t>Cardinal Grosbeak by James Audubon 12 x 16 Print in Black Beveled Frame | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Hunting Gift</t>
         </is>
       </c>
-      <c r="D42" t="n">
+      <c r="E42" t="n">
         <v>2</v>
       </c>
-      <c r="E42" t="n">
+      <c r="F42" t="n">
         <v>54.98</v>
       </c>
     </row>
@@ -1620,18 +1830,23 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>R0U8UMGE34</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
           <t>Rose Breasted Grosbeak by James Audubon 12 x 16 Print Unframed | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Hunting Gift</t>
         </is>
       </c>
-      <c r="D43" t="n">
-        <v>1</v>
-      </c>
       <c r="E43" t="n">
+        <v>1</v>
+      </c>
+      <c r="F43" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -1643,18 +1858,23 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>9YS2RARYZE</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
           <t>American Sparrow Hawk by James Audubon 12 x 16 Print Unframed | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Room Gift</t>
         </is>
       </c>
-      <c r="D44" t="n">
+      <c r="E44" t="n">
         <v>2</v>
       </c>
-      <c r="E44" t="n">
+      <c r="F44" t="n">
         <v>54.98</v>
       </c>
     </row>
@@ -1666,18 +1886,23 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>N6GZGE6M99</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
           <t>American Robin by James Audubon 12 x 16 Print Unframed | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Hunting Gift</t>
         </is>
       </c>
-      <c r="D45" t="n">
+      <c r="E45" t="n">
         <v>2</v>
       </c>
-      <c r="E45" t="n">
+      <c r="F45" t="n">
         <v>54.98</v>
       </c>
     </row>
@@ -1689,18 +1914,23 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>10FDM9EIM7</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
           <t>Baltimore Oriole by James Audubon 12 x 16 Print in Black Beveled Frame | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Hunting Gift</t>
         </is>
       </c>
-      <c r="D46" t="n">
-        <v>1</v>
-      </c>
       <c r="E46" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -1712,18 +1942,23 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>BLM3TSZ0T3</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
           <t>Ruby Throated Humming Bird by James Audubon 12 x 16 Print Unframed | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Print in Wood Frame | Home &amp; Office Hunting Gift</t>
         </is>
       </c>
-      <c r="D47" t="n">
+      <c r="E47" t="n">
         <v>3</v>
       </c>
-      <c r="E47" t="n">
+      <c r="F47" t="n">
         <v>94.97</v>
       </c>
     </row>
@@ -1735,18 +1970,23 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>06L5I0ZAQZ</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
           <t>Mocking Bird by James Audubon 12 x 16 Print Unframed | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Hunting Gift Walls</t>
         </is>
       </c>
-      <c r="D48" t="n">
-        <v>1</v>
-      </c>
       <c r="E48" t="n">
+        <v>1</v>
+      </c>
+      <c r="F48" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -1758,18 +1998,23 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>FYG63JBOS8</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
           <t>Pileated Woodpecker by James Audubon 12 x 16 Print Unframed | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Hunting Gift</t>
         </is>
       </c>
-      <c r="D49" t="n">
+      <c r="E49" t="n">
         <v>2</v>
       </c>
-      <c r="E49" t="n">
+      <c r="F49" t="n">
         <v>54.98</v>
       </c>
     </row>
@@ -1781,18 +2026,23 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>3UUBVEI4MJ</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
           <t>Blue Jay by James Audubon 12 x 16 Print in Black Beveled Frame | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Hunting Gift Walls</t>
         </is>
       </c>
-      <c r="D50" t="n">
-        <v>1</v>
-      </c>
       <c r="E50" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -1804,18 +2054,23 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>7UI3PNJDZ9</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
           <t>Summer or Wood Duck by James Audubon 12 x 16 Print in Black Beveled Frame | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Hunting Gift</t>
         </is>
       </c>
-      <c r="D51" t="n">
-        <v>1</v>
-      </c>
       <c r="E51" t="n">
+        <v>1</v>
+      </c>
+      <c r="F51" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -1827,18 +2082,23 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>DHZLI453XV</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
           <t>American Flamingo by James Audubon 18 x 24 Matted Print in Black Flat Frame | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Print in Wood Frame | Home &amp; Office Hunting Gift</t>
         </is>
       </c>
-      <c r="D52" t="n">
+      <c r="E52" t="n">
         <v>2</v>
       </c>
-      <c r="E52" t="n">
+      <c r="F52" t="n">
         <v>124.98</v>
       </c>
     </row>
@@ -1850,18 +2110,23 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>DX7GWLY93P</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
           <t>Lost Cabin Starry Night Over the Rhone by Vincent Van Gogh | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D53" t="n">
-        <v>1</v>
-      </c>
       <c r="E53" t="n">
+        <v>1</v>
+      </c>
+      <c r="F53" t="n">
         <v>32.99</v>
       </c>
     </row>
@@ -1873,18 +2138,23 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>64FV24KETV</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
           <t>Lost Cabin Skull with Burning Cigarette by Vincent Van Gogh | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D54" t="n">
-        <v>1</v>
-      </c>
       <c r="E54" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" t="n">
         <v>32.99</v>
       </c>
     </row>
@@ -1896,18 +2166,23 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>E49WBZQ773</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
           <t>Wild Turkey by James Audubon 12 x 16 Print Unframed | Framed Wall Art Decor | Fine Artwork Painting Reproduction | Gallery Prints in Wood Frame | Home &amp; Office Hunting Gift</t>
         </is>
       </c>
-      <c r="D55" t="n">
+      <c r="E55" t="n">
         <v>2</v>
       </c>
-      <c r="E55" t="n">
+      <c r="F55" t="n">
         <v>29.98</v>
       </c>
     </row>
@@ -1919,18 +2194,23 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>DNBG2AM807</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
           <t>Lost Cabin Great Blue Heron by James Audubon | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Hunting Gift | Image: 14 x 20 Frame: 20.5 x 26.5</t>
         </is>
       </c>
-      <c r="D56" t="n">
-        <v>1</v>
-      </c>
       <c r="E56" t="n">
+        <v>1</v>
+      </c>
+      <c r="F56" t="n">
         <v>84.98999999999999</v>
       </c>
     </row>
@@ -1942,18 +2222,23 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>PV2WAUMIGN</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
           <t>Lost Cabin American Flamingo by James Audubon | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Hunting Gift | Image: 12 x 16 No Frame</t>
         </is>
       </c>
-      <c r="D57" t="n">
-        <v>1</v>
-      </c>
       <c r="E57" t="n">
+        <v>1</v>
+      </c>
+      <c r="F57" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -1965,18 +2250,23 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>99RXSBWNY5</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
           <t>Baltimore Oriole by James Audubon Framed Print Poster Wall Art Decor | Fine Artwork Painting Reproduction Posters &amp; Pictures | Gallery Prints in Wood Frame | Home &amp; Office for Bedroom &amp; Living Room</t>
         </is>
       </c>
-      <c r="D58" t="n">
+      <c r="E58" t="n">
         <v>2</v>
       </c>
-      <c r="E58" t="n">
+      <c r="F58" t="n">
         <v>29.98</v>
       </c>
     </row>
@@ -1988,18 +2278,23 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
+          <t>3H2D0N9ZVO</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C59" t="inlineStr">
+      <c r="D59" t="inlineStr">
         <is>
           <t>Lost Cabin Saved by Edwin Henry Landseer | Canvas Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 16x24 Frame: 18x26</t>
         </is>
       </c>
-      <c r="D59" t="n">
+      <c r="E59" t="n">
         <v>3</v>
       </c>
-      <c r="E59" t="n">
+      <c r="F59" t="n">
         <v>169.97</v>
       </c>
     </row>
@@ -2011,18 +2306,23 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>JMX2HBQ41X</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
+      <c r="D60" t="inlineStr">
         <is>
           <t>Lost Cabin Among the Waves by Ivan Aivazovsky | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D60" t="n">
-        <v>1</v>
-      </c>
       <c r="E60" t="n">
+        <v>1</v>
+      </c>
+      <c r="F60" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -2034,18 +2334,23 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
+          <t>914FZD7BUH</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C61" t="inlineStr">
+      <c r="D61" t="inlineStr">
         <is>
           <t>Lost Cabin A Mermaid 1900 by John William Waterhouse | Print Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 Frame: 14x20</t>
         </is>
       </c>
-      <c r="D61" t="n">
-        <v>1</v>
-      </c>
       <c r="E61" t="n">
+        <v>1</v>
+      </c>
+      <c r="F61" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2057,18 +2362,23 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>WFND7IBD9H</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
           <t>Lost Cabin Gather Ye Rosebuds While Ye May by John William Waterhouse | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor | Image: 14x20 Frame: 20.5x26.5</t>
         </is>
       </c>
-      <c r="D62" t="n">
-        <v>1</v>
-      </c>
       <c r="E62" t="n">
+        <v>1</v>
+      </c>
+      <c r="F62" t="n">
         <v>84.98999999999999</v>
       </c>
     </row>
@@ -2080,18 +2390,23 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>28Z6YZFT3W</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D63" t="inlineStr">
+        <is>
           <t>Lost Cabin Sailboat at Le Petit Gennevilliers by Claude Monet | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 19x27 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D63" t="n">
+      <c r="E63" t="n">
         <v>4</v>
       </c>
-      <c r="E63" t="n">
+      <c r="F63" t="n">
         <v>509.98</v>
       </c>
     </row>
@@ -2103,18 +2418,23 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>5GNUPPGHFY</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D64" t="inlineStr">
+        <is>
           <t>Lost Cabin Triumph of Bacchus by Diego Velazquez | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D64" t="n">
+      <c r="E64" t="n">
         <v>2</v>
       </c>
-      <c r="E64" t="n">
+      <c r="F64" t="n">
         <v>65.98</v>
       </c>
     </row>
@@ -2126,18 +2446,23 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>EQI9TQVC8C</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D65" t="inlineStr">
+        <is>
           <t>Lost Cabin Crucifixion of Saint Peter by Caravaggio | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D65" t="n">
+      <c r="E65" t="n">
         <v>2</v>
       </c>
-      <c r="E65" t="n">
+      <c r="F65" t="n">
         <v>40.98</v>
       </c>
     </row>
@@ -2149,18 +2474,23 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>8FVV3B0NFK</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D66" t="inlineStr">
+        <is>
           <t>Lost Cabin Young Woman in the Garden by Edouard Manet | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 No Frame</t>
         </is>
       </c>
-      <c r="D66" t="n">
-        <v>1</v>
-      </c>
       <c r="E66" t="n">
+        <v>1</v>
+      </c>
+      <c r="F66" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -2172,18 +2502,23 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>K3EZMKEAD3</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D67" t="inlineStr">
+        <is>
           <t>Lost Cabin Return of the Prodigal Son by Van Rjin Rembrandt | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D67" t="n">
-        <v>1</v>
-      </c>
       <c r="E67" t="n">
+        <v>1</v>
+      </c>
+      <c r="F67" t="n">
         <v>64.98999999999999</v>
       </c>
     </row>
@@ -2195,18 +2530,23 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>4FWPS4JWPDx2</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D68" t="inlineStr">
+        <is>
           <t>Lost Cabin The Wanderer Above the Sea of Fog by Caspar David Friedrich | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D68" t="n">
-        <v>1</v>
-      </c>
       <c r="E68" t="n">
+        <v>1</v>
+      </c>
+      <c r="F68" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2218,18 +2558,23 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>K3EZMKEAD3x2</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D69" t="inlineStr">
+        <is>
           <t>Lost Cabin Return of the Prodigal Son by Van Rjin Rembrandt | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D69" t="n">
-        <v>1</v>
-      </c>
       <c r="E69" t="n">
+        <v>1</v>
+      </c>
+      <c r="F69" t="n">
         <v>32.99</v>
       </c>
     </row>
@@ -2241,18 +2586,23 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>4FWPS4JWPD</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D70" t="inlineStr">
+        <is>
           <t>Lost Cabin The Wanderer Above the Sea of Fog by Caspar David Friedrich | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D70" t="n">
-        <v>1</v>
-      </c>
       <c r="E70" t="n">
+        <v>1</v>
+      </c>
+      <c r="F70" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2264,18 +2614,23 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>TXZT5O7EJW</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D71" t="inlineStr">
+        <is>
           <t>Lost Cabin Vase with Poppies Cornflowers Peonies &amp; Chrysanthemums by Vincent Van Gogh | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D71" t="n">
+      <c r="E71" t="n">
         <v>3</v>
       </c>
-      <c r="E71" t="n">
+      <c r="F71" t="n">
         <v>229.97</v>
       </c>
     </row>
@@ -2287,18 +2642,23 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>WIOK9FFUV1</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D72" t="inlineStr">
+        <is>
           <t>Lost Cabin Alexander Hamilton in the Uniform of the New York Artillery by Alonzo Chappel | Print in Black Flat Frame | Fine Artwork Painting Reproduction Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D72" t="n">
-        <v>1</v>
-      </c>
       <c r="E72" t="n">
+        <v>1</v>
+      </c>
+      <c r="F72" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2310,18 +2670,23 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>5FGFO99WFL</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D73" t="inlineStr">
+        <is>
           <t>Lost Cabin Woman Baking Bread by Jean Francois Millet | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D73" t="n">
-        <v>1</v>
-      </c>
       <c r="E73" t="n">
+        <v>1</v>
+      </c>
+      <c r="F73" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2333,18 +2698,23 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>MCZO8U7YN2</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D74" t="inlineStr">
+        <is>
           <t>Lost Cabin Alexis De Tocqueville by Theodore Chasseriau | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 No Frame</t>
         </is>
       </c>
-      <c r="D74" t="n">
-        <v>1</v>
-      </c>
       <c r="E74" t="n">
+        <v>1</v>
+      </c>
+      <c r="F74" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -2356,18 +2726,23 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>VFPL7D3Z65</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D75" t="inlineStr">
+        <is>
           <t>Lost Cabin St Paul in Prison by Van Rjin Rembrandt | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D75" t="n">
-        <v>1</v>
-      </c>
       <c r="E75" t="n">
+        <v>1</v>
+      </c>
+      <c r="F75" t="n">
         <v>64.98999999999999</v>
       </c>
     </row>
@@ -2379,18 +2754,23 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>SLHM282615</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D76" t="inlineStr">
+        <is>
           <t>Lost Cabin An Evening at Home 1888 by Edward Poynter | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D76" t="n">
+      <c r="E76" t="n">
         <v>2</v>
       </c>
-      <c r="E76" t="n">
+      <c r="F76" t="n">
         <v>54.98</v>
       </c>
     </row>
@@ -2402,18 +2782,23 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>UI87T0O52H</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D77" t="inlineStr">
+        <is>
           <t>Lost Cabin Flight Into Egypt by Henry Ossawa Tanner | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D77" t="n">
-        <v>1</v>
-      </c>
       <c r="E77" t="n">
+        <v>1</v>
+      </c>
+      <c r="F77" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2425,18 +2810,23 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>S7468R0H9Y</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D78" t="inlineStr">
+        <is>
           <t>Lost Cabin Vengeance Is Sworn 1851 by Francesco Paolo Hayez | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D78" t="n">
-        <v>1</v>
-      </c>
       <c r="E78" t="n">
+        <v>1</v>
+      </c>
+      <c r="F78" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2448,18 +2838,23 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>F3YWU4ME6U</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D79" t="inlineStr">
+        <is>
           <t>Lost Cabin A Bend in the Road by Paul Cezanne | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D79" t="n">
-        <v>1</v>
-      </c>
       <c r="E79" t="n">
+        <v>1</v>
+      </c>
+      <c r="F79" t="n">
         <v>89.98999999999999</v>
       </c>
     </row>
@@ -2471,18 +2866,23 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>EFDQ4K355Y</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D80" t="inlineStr">
+        <is>
           <t>Lost Cabin Dickens Dream by Robert William Buss | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D80" t="n">
-        <v>1</v>
-      </c>
       <c r="E80" t="n">
+        <v>1</v>
+      </c>
+      <c r="F80" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2494,18 +2894,23 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>FCES4B4Y9N</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D81" t="inlineStr">
+        <is>
           <t>Lost Cabin Ballet Rehearsal by Edgar Degas | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 No Frame</t>
         </is>
       </c>
-      <c r="D81" t="n">
+      <c r="E81" t="n">
         <v>2</v>
       </c>
-      <c r="E81" t="n">
+      <c r="F81" t="n">
         <v>32.98</v>
       </c>
     </row>
@@ -2517,18 +2922,23 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>CT1SEBSGBZ</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D82" t="inlineStr">
+        <is>
           <t>Lost Cabin The Son of Man by Rene Magritte | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D82" t="n">
-        <v>1</v>
-      </c>
       <c r="E82" t="n">
+        <v>1</v>
+      </c>
+      <c r="F82" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2540,18 +2950,23 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>DZPIZ3VRSV</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D83" t="inlineStr">
+        <is>
           <t>Lost Cabin The Human Condition by Rene Magritte | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D83" t="n">
+      <c r="E83" t="n">
         <v>2</v>
       </c>
-      <c r="E83" t="n">
+      <c r="F83" t="n">
         <v>54.98</v>
       </c>
     </row>
@@ -2563,18 +2978,23 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>55YY1HDB82</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D84" t="inlineStr">
+        <is>
           <t>Lost Cabin Three Dancers in an Exercise Hall by Edgar Degas | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 No Frame</t>
         </is>
       </c>
-      <c r="D84" t="n">
-        <v>1</v>
-      </c>
       <c r="E84" t="n">
+        <v>1</v>
+      </c>
+      <c r="F84" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -2586,18 +3006,23 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>8NW6TGMDPX</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D85" t="inlineStr">
+        <is>
           <t>Lost Cabin Still Life of Fruit &amp; Urn 1878 by T. C. Steele | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 No Frame</t>
         </is>
       </c>
-      <c r="D85" t="n">
-        <v>1</v>
-      </c>
       <c r="E85" t="n">
+        <v>1</v>
+      </c>
+      <c r="F85" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -2609,18 +3034,23 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>5F36IZAYH6</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D86" t="inlineStr">
+        <is>
           <t>Lost Cabin A Ship at Sea Sunset by Edward Moran | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D86" t="n">
-        <v>1</v>
-      </c>
       <c r="E86" t="n">
+        <v>1</v>
+      </c>
+      <c r="F86" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2632,18 +3062,23 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>2FDVIQR5UE</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D87" t="inlineStr">
+        <is>
           <t>Lost Cabin Young Lady with Gloves by Tamara de Lempicka | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 No Frame</t>
         </is>
       </c>
-      <c r="D87" t="n">
-        <v>1</v>
-      </c>
       <c r="E87" t="n">
+        <v>1</v>
+      </c>
+      <c r="F87" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -2655,18 +3090,23 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>2XK0UICJRP</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
           <t>Lost Cabin The Midnight Ride of Paul Revere by Grant Wood | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D88" t="n">
-        <v>1</v>
-      </c>
       <c r="E88" t="n">
+        <v>1</v>
+      </c>
+      <c r="F88" t="n">
         <v>89.98999999999999</v>
       </c>
     </row>
@@ -2678,18 +3118,23 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>1RCDJ426MR</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
           <t>Lost Cabin Temptation by William Bouguereau | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D89" t="n">
-        <v>1</v>
-      </c>
       <c r="E89" t="n">
+        <v>1</v>
+      </c>
+      <c r="F89" t="n">
         <v>89.98999999999999</v>
       </c>
     </row>
@@ -2701,18 +3146,23 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>AIBJ5B5FUN</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
           <t>Lost Cabin The Boats by Claude Monet | Canvas in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 24x32 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D90" t="n">
+      <c r="E90" t="n">
         <v>3</v>
       </c>
-      <c r="E90" t="n">
+      <c r="F90" t="n">
         <v>389.97</v>
       </c>
     </row>
@@ -2724,18 +3174,23 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>ODF0YBHW76</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
           <t>The Sleeper by Tamara de Lempicka Framed Print Poster Wall Art Decor | Fine Artwork Painting Reproduction Posters &amp; Pictures | Gallery Prints in Wood Frame | Home &amp; Office for Bedroom &amp; Living Room</t>
         </is>
       </c>
-      <c r="D91" t="n">
-        <v>1</v>
-      </c>
       <c r="E91" t="n">
+        <v>1</v>
+      </c>
+      <c r="F91" t="n">
         <v>84.98999999999999</v>
       </c>
     </row>
@@ -2747,18 +3202,23 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>UT4C1G6Y68</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D92" t="inlineStr">
+        <is>
           <t>Lost Cabin Orpheus and Eurydice by George Frederic Watts | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D92" t="n">
-        <v>1</v>
-      </c>
       <c r="E92" t="n">
+        <v>1</v>
+      </c>
+      <c r="F92" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2770,18 +3230,23 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>AJC7JL32D3</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D93" t="inlineStr">
+        <is>
           <t>Lost Cabin The Cemetery Entrance 1825 by Caspar David Friedrich | Canvas in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 24x32 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D93" t="n">
-        <v>1</v>
-      </c>
       <c r="E93" t="n">
+        <v>1</v>
+      </c>
+      <c r="F93" t="n">
         <v>94.98999999999999</v>
       </c>
     </row>
@@ -2793,18 +3258,23 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>9C8BXAPHL9</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D94" t="inlineStr">
+        <is>
           <t>Lost Cabin Chez Tortoni by Edouard Manet | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D94" t="n">
-        <v>1</v>
-      </c>
       <c r="E94" t="n">
+        <v>1</v>
+      </c>
+      <c r="F94" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -2816,18 +3286,23 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>65OW1ATU9R</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D95" t="inlineStr">
+        <is>
           <t>Lost Cabin Landscape Near Montecarlo by Claude Monet | Canvas in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 24x32 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D95" t="n">
-        <v>1</v>
-      </c>
       <c r="E95" t="n">
+        <v>1</v>
+      </c>
+      <c r="F95" t="n">
         <v>129.99</v>
       </c>
     </row>
@@ -2839,18 +3314,23 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>E5DEULU4GN</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D96" t="inlineStr">
+        <is>
           <t>Lost Cabin Las Meninas by Diego Velazquez | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D96" t="n">
-        <v>1</v>
-      </c>
       <c r="E96" t="n">
+        <v>1</v>
+      </c>
+      <c r="F96" t="n">
         <v>32.99</v>
       </c>
     </row>
@@ -2862,18 +3342,23 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>9FTMLWNLRX</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D97" t="inlineStr">
+        <is>
           <t>Lost Cabin The Promenade Woman with a Parasol by Claude Monet | Canvas in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 24x32 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D97" t="n">
-        <v>1</v>
-      </c>
       <c r="E97" t="n">
+        <v>1</v>
+      </c>
+      <c r="F97" t="n">
         <v>129.99</v>
       </c>
     </row>
@@ -2885,18 +3370,23 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>YCJ12ML9L4</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D98" t="inlineStr">
+        <is>
           <t>Lost Cabin Bridges Across the Seine by Vincent Van Gogh | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D98" t="n">
-        <v>1</v>
-      </c>
       <c r="E98" t="n">
+        <v>1</v>
+      </c>
+      <c r="F98" t="n">
         <v>89.98999999999999</v>
       </c>
     </row>
@@ -2908,18 +3398,23 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>CSJULCSTOG</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D99" t="inlineStr">
+        <is>
           <t>Lost Cabin Cafe Terrace at Night by Vincent Van Gogh | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 No Frame</t>
         </is>
       </c>
-      <c r="D99" t="n">
-        <v>1</v>
-      </c>
       <c r="E99" t="n">
+        <v>1</v>
+      </c>
+      <c r="F99" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -2931,18 +3426,23 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
+          <t>54OB1TU2L1</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C100" t="inlineStr">
+      <c r="D100" t="inlineStr">
         <is>
           <t>Lost Cabin Pirates Fight in Who Shall Be Captain by Howard Pyle | Canvas Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 16x24 Frame: 18x26</t>
         </is>
       </c>
-      <c r="D100" t="n">
-        <v>1</v>
-      </c>
       <c r="E100" t="n">
+        <v>1</v>
+      </c>
+      <c r="F100" t="n">
         <v>89.98999999999999</v>
       </c>
     </row>
@@ -2954,18 +3454,23 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
+          <t>4VT0WF6IV9</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C101" t="inlineStr">
+      <c r="D101" t="inlineStr">
         <is>
           <t>Lost Cabin General George Washington at Trenton 1792 by John Trumbull | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D101" t="n">
-        <v>1</v>
-      </c>
       <c r="E101" t="n">
+        <v>1</v>
+      </c>
+      <c r="F101" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -2977,18 +3482,23 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>6Q908OGYAK</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
           <t>Lost Cabin The Piano Lesson by Pierre Renoir | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D102" t="n">
-        <v>1</v>
-      </c>
       <c r="E102" t="n">
+        <v>1</v>
+      </c>
+      <c r="F102" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -3000,18 +3510,23 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
+          <t>1LBRRFCTZZ</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C103" t="inlineStr">
+      <c r="D103" t="inlineStr">
         <is>
           <t>Lost Cabin Nude Descending a Staircase Number 2 by Marcel Duchamp | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D103" t="n">
-        <v>1</v>
-      </c>
       <c r="E103" t="n">
+        <v>1</v>
+      </c>
+      <c r="F103" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -3023,18 +3538,23 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>Q2RQ2W8FCZ</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
           <t>Lost Cabin Algerian Girl by Pierre Renoir | Canvas in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 24x32 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D104" t="n">
-        <v>1</v>
-      </c>
       <c r="E104" t="n">
+        <v>1</v>
+      </c>
+      <c r="F104" t="n">
         <v>129.99</v>
       </c>
     </row>
@@ -3046,18 +3566,23 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>CTBZP71VOM</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
           <t>Lost Cabin Girls at the Piano by Pierre Renoir | Canvas in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 24x32 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D105" t="n">
+      <c r="E105" t="n">
         <v>2</v>
       </c>
-      <c r="E105" t="n">
+      <c r="F105" t="n">
         <v>112.98</v>
       </c>
     </row>
@@ -3069,18 +3594,23 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>LAHGDDGZOJ</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
           <t>Lost Cabin Odalisque by Pierre Renoir | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 No Frame</t>
         </is>
       </c>
-      <c r="D106" t="n">
-        <v>1</v>
-      </c>
       <c r="E106" t="n">
+        <v>1</v>
+      </c>
+      <c r="F106" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -3092,18 +3622,23 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>TDMKQCA3GR</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
           <t>Lost Cabin Garden In The Rue Cortot Montmartre 1876 by Pierre Renoir | Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D107" t="n">
-        <v>1</v>
-      </c>
       <c r="E107" t="n">
+        <v>1</v>
+      </c>
+      <c r="F107" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -3115,18 +3650,23 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
+          <t>SOCHY6QDZR</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
           <t>2x3</t>
         </is>
       </c>
-      <c r="C108" t="inlineStr">
+      <c r="D108" t="inlineStr">
         <is>
           <t>Lost Cabin Three Worlds by M.C. Escher | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster | Image: 12x18 No Frame</t>
         </is>
       </c>
-      <c r="D108" t="n">
-        <v>1</v>
-      </c>
       <c r="E108" t="n">
+        <v>1</v>
+      </c>
+      <c r="F108" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -3138,18 +3678,23 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>SKB9HDO07L</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
           <t>Lost Cabin Two Statues by Salvador Dali | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 14x20 Frame: 20.5x26.5</t>
         </is>
       </c>
-      <c r="D109" t="n">
-        <v>1</v>
-      </c>
       <c r="E109" t="n">
+        <v>1</v>
+      </c>
+      <c r="F109" t="n">
         <v>84.98999999999999</v>
       </c>
     </row>
@@ -3161,18 +3706,23 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>WZ7KL28BNC</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
           <t>Lost Cabin Dream 1932 by Pablo Picasso | Print in Black Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D110" t="n">
-        <v>1</v>
-      </c>
       <c r="E110" t="n">
+        <v>1</v>
+      </c>
+      <c r="F110" t="n">
         <v>32.99</v>
       </c>
     </row>
@@ -3184,18 +3734,23 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>WF670K55MX</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
           <t>Lost Cabin Woman with Mustard Pot 1910 by Pablo Picasso | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D111" t="n">
+      <c r="E111" t="n">
         <v>5</v>
       </c>
-      <c r="E111" t="n">
+      <c r="F111" t="n">
         <v>203.95</v>
       </c>
     </row>
@@ -3207,18 +3762,23 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>56XFU9MO0G</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
           <t>Lost Cabin Girl with a Mandolin 1910 by Pablo Picasso | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 14x20 Frame: 20.5x26.5</t>
         </is>
       </c>
-      <c r="D112" t="n">
+      <c r="E112" t="n">
         <v>2</v>
       </c>
-      <c r="E112" t="n">
+      <c r="F112" t="n">
         <v>134.98</v>
       </c>
     </row>
@@ -3230,18 +3790,23 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>O9MIJT3A85</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
           <t>Lost Cabin Girl before a Mirror by Pablo Picasso | Print in Black Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D113" t="n">
+      <c r="E113" t="n">
         <v>5</v>
       </c>
-      <c r="E113" t="n">
+      <c r="F113" t="n">
         <v>273.95</v>
       </c>
     </row>
@@ -3253,18 +3818,23 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>7ABP9A7TQD</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
           <t>Lost Cabin The Weeping Woman 1937 by Pablo Picasso | Print in Black Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D114" t="n">
-        <v>1</v>
-      </c>
       <c r="E114" t="n">
+        <v>1</v>
+      </c>
+      <c r="F114" t="n">
         <v>32.99</v>
       </c>
     </row>
@@ -3276,18 +3846,23 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>WCEBFZ63OY</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
           <t>Lost Cabin Dream Caused by The Flight by Salvador Dali | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 14x20 Frame: 20.5x26.5</t>
         </is>
       </c>
-      <c r="D115" t="n">
+      <c r="E115" t="n">
         <v>2</v>
       </c>
-      <c r="E115" t="n">
+      <c r="F115" t="n">
         <v>77.97999999999999</v>
       </c>
     </row>
@@ -3299,18 +3874,23 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>RETRO3-LEAHIZYPG1</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
           <t>Park Central Hotel Moon Over Miami by Larry Grossman Framed Canvas Wall Art Decor | Canvases &amp; Pictures | Artwork for Home &amp; Living Room Wall Decor</t>
         </is>
       </c>
-      <c r="D116" t="n">
-        <v>1</v>
-      </c>
       <c r="E116" t="n">
+        <v>1</v>
+      </c>
+      <c r="F116" t="n">
         <v>89.98999999999999</v>
       </c>
     </row>
@@ -3322,18 +3902,23 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>Z20OZG8JLR</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
           <t>Lost Cabin Champagne De Rochegre by Leonetto Cappiello | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 14x20 Frame: 20.5x26.5</t>
         </is>
       </c>
-      <c r="D117" t="n">
+      <c r="E117" t="n">
         <v>2</v>
       </c>
-      <c r="E117" t="n">
+      <c r="F117" t="n">
         <v>84.97999999999999</v>
       </c>
     </row>
@@ -3345,18 +3930,23 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>O1HBG1SLAY</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
           <t>Lost Cabin Absinthe by Leonetto Cappiello | Matted Print in Black Flat Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 14x20 Frame: 20.5x26.5</t>
         </is>
       </c>
-      <c r="D118" t="n">
-        <v>1</v>
-      </c>
       <c r="E118" t="n">
+        <v>1</v>
+      </c>
+      <c r="F118" t="n">
         <v>69.98999999999999</v>
       </c>
     </row>
@@ -3368,18 +3958,23 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>A227DNP1YI</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
           <t>Lost Cabin Asti Cinzano by Leonetto Cappiello | Matted Print in Black Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 19x27 Frame: 28x36</t>
         </is>
       </c>
-      <c r="D119" t="n">
+      <c r="E119" t="n">
         <v>2</v>
       </c>
-      <c r="E119" t="n">
+      <c r="F119" t="n">
         <v>209.99</v>
       </c>
     </row>
@@ -3391,18 +3986,23 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>UHCRJDH7K1</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
           <t>Lost Cabin Aix Les Bains by Leonetto Cappiello | Canvas in Gold Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 18x24 Frame: 22x28</t>
         </is>
       </c>
-      <c r="D120" t="n">
-        <v>1</v>
-      </c>
       <c r="E120" t="n">
+        <v>1</v>
+      </c>
+      <c r="F120" t="n">
         <v>64.98999999999999</v>
       </c>
     </row>
@@ -3414,18 +4014,23 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>ZH668SNZ84</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
           <t>Lost Cabin Cognac Monnet by Leonetto Cappiello | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 No Frame</t>
         </is>
       </c>
-      <c r="D121" t="n">
+      <c r="E121" t="n">
         <v>2</v>
       </c>
-      <c r="E121" t="n">
+      <c r="F121" t="n">
         <v>22.98</v>
       </c>
     </row>
@@ -3437,18 +4042,23 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>X13KMVRKHX</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
           <t>Lost Cabin Isolabella by Leonetto Cappiello | Print in Black Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 14.5x18.5</t>
         </is>
       </c>
-      <c r="D122" t="n">
-        <v>1</v>
-      </c>
       <c r="E122" t="n">
+        <v>1</v>
+      </c>
+      <c r="F122" t="n">
         <v>32.99</v>
       </c>
     </row>
@@ -3460,18 +4070,23 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>5LWX44MG6T</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
           <t>Lost Cabin Pates Baroni by Leonetto Cappiello | Print in Black Beveled Frame | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 Frame: 14.5x18.5</t>
         </is>
       </c>
-      <c r="D123" t="n">
-        <v>1</v>
-      </c>
       <c r="E123" t="n">
+        <v>1</v>
+      </c>
+      <c r="F123" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -3483,18 +4098,23 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>2E59WZV7TU</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
           <t>Lost Cabin Cafe Martin by Leonetto Cappiello | Print Unframed | Fine Artwork Painting Reproduction | Framed Wall Art Decor Poster Gift | Image: 12x16 No Frame</t>
         </is>
       </c>
-      <c r="D124" t="n">
-        <v>1</v>
-      </c>
       <c r="E124" t="n">
+        <v>1</v>
+      </c>
+      <c r="F124" t="n">
         <v>14.99</v>
       </c>
     </row>
@@ -3506,18 +4126,23 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>6HKBNJ635L</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
           <t>Lost Cabin White Poodle in a Punt by George Stubbs Framed Poster Wall Art Decor Print | Posters &amp; Prints | Horses, Dogs &amp; Wildlife Artwork for Home &amp; Game Room Wall Decor</t>
         </is>
       </c>
-      <c r="D125" t="n">
-        <v>1</v>
-      </c>
       <c r="E125" t="n">
+        <v>1</v>
+      </c>
+      <c r="F125" t="n">
         <v>39.99</v>
       </c>
     </row>
@@ -3529,18 +4154,23 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>ZRBMVBB1E2</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
           <t>Lost Cabin Autumn on the Seine at Argenteuil by Claude Monet Framed Poster Wall Art Decor Print | Posters &amp; Prints | nature, landscapes &amp; botanical Artwork for Home &amp; Living Room Wall Decor</t>
         </is>
       </c>
-      <c r="D126" t="n">
+      <c r="E126" t="n">
         <v>2</v>
       </c>
-      <c r="E126" t="n">
+      <c r="F126" t="n">
         <v>40.98</v>
       </c>
     </row>
@@ -3552,18 +4182,23 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>191FPAUNQR</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
           <t>Lost Cabin Poplars on the Epte by Claude Monet Framed Poster Wall Art Decor Print | Posters &amp; Prints | nature, landscapes &amp; botanical Artwork for Home &amp; Living Room Wall Decor</t>
         </is>
       </c>
-      <c r="D127" t="n">
+      <c r="E127" t="n">
         <v>2</v>
       </c>
-      <c r="E127" t="n">
+      <c r="F127" t="n">
         <v>40.98</v>
       </c>
     </row>
@@ -3575,18 +4210,23 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>0DH92SWDXP</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
           <t>Woman in Hat and Fur Collar 1937 by Pablo Picasso Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D128" t="n">
+      <c r="E128" t="n">
         <v>2</v>
       </c>
-      <c r="E128" t="n">
+      <c r="F128" t="n">
         <v>15.98</v>
       </c>
     </row>
@@ -3598,18 +4238,23 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>XU6J1FY5AJ</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
           <t>Grove of Olive Trees by Claude Monet Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D129" t="n">
-        <v>1</v>
-      </c>
       <c r="E129" t="n">
+        <v>1</v>
+      </c>
+      <c r="F129" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -3621,18 +4266,23 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>HSASI7911R</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
           <t>Women in the Garden by Claude Monet Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D130" t="n">
+      <c r="E130" t="n">
         <v>2</v>
       </c>
-      <c r="E130" t="n">
+      <c r="F130" t="n">
         <v>25.98</v>
       </c>
     </row>
@@ -3644,18 +4294,23 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>DKZIVB1UR0</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
           <t>The Manneport by Claude Monet Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D131" t="n">
-        <v>1</v>
-      </c>
       <c r="E131" t="n">
+        <v>1</v>
+      </c>
+      <c r="F131" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -3667,18 +4322,23 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>P6LE8HN7GJ</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
           <t>Belshazzars Feast by Van Rjin Rembrandt Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D132" t="n">
+      <c r="E132" t="n">
         <v>2</v>
       </c>
-      <c r="E132" t="n">
+      <c r="F132" t="n">
         <v>15.98</v>
       </c>
     </row>
@@ -3690,18 +4350,23 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>J52RLCNWYB</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
           <t>Low Tide at Pourville by Claude Monet Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D133" t="n">
-        <v>1</v>
-      </c>
       <c r="E133" t="n">
+        <v>1</v>
+      </c>
+      <c r="F133" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -3713,18 +4378,23 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>6R2VJ6RCJG</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
           <t>Saint Lazare Station by Claude Monet Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D134" t="n">
+      <c r="E134" t="n">
         <v>2</v>
       </c>
-      <c r="E134" t="n">
+      <c r="F134" t="n">
         <v>15.98</v>
       </c>
     </row>
@@ -3736,18 +4406,23 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>EXSU8HZJQB</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
           <t>Boulevard of Capucines by Claude Monet Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D135" t="n">
-        <v>1</v>
-      </c>
       <c r="E135" t="n">
+        <v>1</v>
+      </c>
+      <c r="F135" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -3759,18 +4434,23 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>QF3L30N7YV</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
           <t>Farm Garden with Crucifix by Gustav Klimt Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D136" t="n">
-        <v>1</v>
-      </c>
       <c r="E136" t="n">
+        <v>1</v>
+      </c>
+      <c r="F136" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -3782,18 +4462,23 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>YLMMIL9UMG</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
           <t>Aristotle with a Bust of Homer 2 by Van Rjin Rembrandt Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D137" t="n">
-        <v>1</v>
-      </c>
       <c r="E137" t="n">
+        <v>1</v>
+      </c>
+      <c r="F137" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -3805,18 +4490,23 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>4L5GQG1OP2</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
           <t>Gardeners House at Antibes by Claude Monet Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D138" t="n">
-        <v>1</v>
-      </c>
       <c r="E138" t="n">
+        <v>1</v>
+      </c>
+      <c r="F138" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -3828,18 +4518,23 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>XAUJJWB6U0</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
           <t>A Pair of Shoes by Vincent Van Gogh Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D139" t="n">
-        <v>1</v>
-      </c>
       <c r="E139" t="n">
+        <v>1</v>
+      </c>
+      <c r="F139" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -3851,18 +4546,23 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>WRMF1HC2LH</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
           <t>The Sunflower 1907 by Gustav Klimt Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D140" t="n">
-        <v>1</v>
-      </c>
       <c r="E140" t="n">
+        <v>1</v>
+      </c>
+      <c r="F140" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -3874,18 +4574,23 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>EV05X96QP4</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
           <t>Death &amp; Life by Gustav Klimt Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D141" t="n">
-        <v>1</v>
-      </c>
       <c r="E141" t="n">
+        <v>1</v>
+      </c>
+      <c r="F141" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -3897,18 +4602,23 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>L8ZTGRGU07</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
           <t>Avenue with Flowering Chestnut Trees at Arles by Vincent Van Gogh Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D142" t="n">
-        <v>1</v>
-      </c>
       <c r="E142" t="n">
+        <v>1</v>
+      </c>
+      <c r="F142" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -3920,18 +4630,23 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>QJEEV6XUMA</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
           <t>Bowl with Peonies &amp; Roses 1886 by Vincent Van Gogh Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D143" t="n">
-        <v>1</v>
-      </c>
       <c r="E143" t="n">
+        <v>1</v>
+      </c>
+      <c r="F143" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -3943,18 +4658,23 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>XF7F7FY13B</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
           <t>Girl in the Woods by Vincent Van Gogh Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D144" t="n">
-        <v>1</v>
-      </c>
       <c r="E144" t="n">
+        <v>1</v>
+      </c>
+      <c r="F144" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -3966,18 +4686,23 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>IU68PURSEV</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
           <t>Church in Cassone by Gustav Klimt Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D145" t="n">
-        <v>1</v>
-      </c>
       <c r="E145" t="n">
+        <v>1</v>
+      </c>
+      <c r="F145" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -3989,18 +4714,23 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>L4XPUACHFX</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
           <t>Autumn Landscape by Vincent Van Gogh Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor Gift for Men &amp; Women Living Room, Bedroom, Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D146" t="n">
-        <v>1</v>
-      </c>
       <c r="E146" t="n">
+        <v>1</v>
+      </c>
+      <c r="F146" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -4012,18 +4742,23 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>AVOI28NT2B</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
           <t>Florio Cinzano by Leonetto Cappiello Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor LivingRoom Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D147" t="n">
-        <v>1</v>
-      </c>
       <c r="E147" t="n">
+        <v>1</v>
+      </c>
+      <c r="F147" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -4035,18 +4770,23 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>OCLLEYTCOH</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
           <t>Il Cigno Di by Leonetto Cappiello Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor LivingRoom Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D148" t="n">
-        <v>1</v>
-      </c>
       <c r="E148" t="n">
+        <v>1</v>
+      </c>
+      <c r="F148" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -4058,18 +4798,23 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>Y0P10IYRD1</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
           <t>A Road in Louveciennes by Pierre Renoir Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor LivingRoom Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D149" t="n">
+      <c r="E149" t="n">
         <v>3</v>
       </c>
-      <c r="E149" t="n">
+      <c r="F149" t="n">
         <v>23.97</v>
       </c>
     </row>
@@ -4081,18 +4826,23 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>HXHTQ3ABF8</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
           <t>In the Meadow by Pierre Renoir Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor LivingRoom Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D150" t="n">
-        <v>1</v>
-      </c>
       <c r="E150" t="n">
+        <v>1</v>
+      </c>
+      <c r="F150" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -4104,18 +4854,23 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>WYXD9A133A</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
           <t>A Bouquet of Roses by Pierre Renoir Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor LivingRoom Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D151" t="n">
-        <v>1</v>
-      </c>
       <c r="E151" t="n">
+        <v>1</v>
+      </c>
+      <c r="F151" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -4127,18 +4882,23 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>TXJU76MSCY</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
           <t>Edgar Degas the Ballet Class by Edgar Degas Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor LivingRoom Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D152" t="n">
-        <v>1</v>
-      </c>
       <c r="E152" t="n">
+        <v>1</v>
+      </c>
+      <c r="F152" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -4150,18 +4910,23 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>1P58ZOFUIG</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
           <t>Spring Margot Standing in a Garden by Mary Cassatt Premium Poster Print | Fine Artwork Painting Reproduction | Wall Art Decor LivingRoom Office | Image: 9x12 Not Framed</t>
         </is>
       </c>
-      <c r="D153" t="n">
-        <v>1</v>
-      </c>
       <c r="E153" t="n">
+        <v>1</v>
+      </c>
+      <c r="F153" t="n">
         <v>7.99</v>
       </c>
     </row>
@@ -4173,18 +4938,23 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>B2R8ABO1G3</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
           <t>Ball at the Moulin De La Galette by Pierre Renoir Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D154" t="n">
-        <v>1</v>
-      </c>
       <c r="E154" t="n">
+        <v>1</v>
+      </c>
+      <c r="F154" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -4196,18 +4966,23 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>0CAPWZKFZP</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
           <t>Bouquet in Front of a Mirror by Pierre Renoir Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D155" t="n">
-        <v>1</v>
-      </c>
       <c r="E155" t="n">
+        <v>1</v>
+      </c>
+      <c r="F155" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -4219,18 +4994,23 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>MEMO1DRIL3</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
           <t>Dance Class at the Opera by Edgar Degas Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D156" t="n">
+      <c r="E156" t="n">
         <v>2</v>
       </c>
-      <c r="E156" t="n">
+      <c r="F156" t="n">
         <v>35.98</v>
       </c>
     </row>
@@ -4242,18 +5022,23 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>VSX0JAJXTB</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
           <t>The Elephants 1948 by Salvador Dali Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D157" t="n">
-        <v>1</v>
-      </c>
       <c r="E157" t="n">
+        <v>1</v>
+      </c>
+      <c r="F157" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -4265,18 +5050,23 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>27X9CTD1VB</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
           <t>The Rose Garden at Wargemont by Pierre Renoir Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D158" t="n">
-        <v>1</v>
-      </c>
       <c r="E158" t="n">
+        <v>1</v>
+      </c>
+      <c r="F158" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -4288,18 +5078,23 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>OQZUZ1B6ZP</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
           <t>The Mandolin Player by Mary Cassatt Canvas Premium Giclee Art Print Unframed | Fine Artwork Painting Reproduction | Wall Art Decor Canvas Poster Gift | 12x16 Canvas</t>
         </is>
       </c>
-      <c r="D159" t="n">
-        <v>1</v>
-      </c>
       <c r="E159" t="n">
+        <v>1</v>
+      </c>
+      <c r="F159" t="n">
         <v>17.99</v>
       </c>
     </row>
@@ -4311,18 +5106,23 @@
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>00BAYZ1JVJ</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
           <t>Donald Trump Assassination Attempt Fight For America Photo Framed Poster Wall Art Decor Print | Trump Sign Posters &amp; Prints | Office Painting and Portrait Wall Decor | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D160" t="n">
-        <v>1</v>
-      </c>
       <c r="E160" t="n">
+        <v>1</v>
+      </c>
+      <c r="F160" t="n">
         <v>32.99</v>
       </c>
     </row>
@@ -4334,18 +5134,23 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>4x3</t>
+          <t>I643J1DGCT</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
         <is>
+          <t>4x3</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
           <t>Donald Trump Rally Shooting Fight For Freedom Framed Poster Wall Art Decor Print | Trump Sign Posters &amp; Prints | Bedroom Painting and Portrait Wall Decor | Image: 12x16 Frame: 13.5x17.5</t>
         </is>
       </c>
-      <c r="D161" t="n">
-        <v>1</v>
-      </c>
       <c r="E161" t="n">
+        <v>1</v>
+      </c>
+      <c r="F161" t="n">
         <v>32.99</v>
       </c>
     </row>

</xml_diff>